<commit_message>
added some repairs to neo4j models
</commit_message>
<xml_diff>
--- a/RSB criteria.xlsx
+++ b/RSB criteria.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmamartin\Projects\curriculumTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4E76788-42B7-4FE4-B515-71B1592B6BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51DF9FC-0B4C-4B01-8D04-A41B035361EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="2865" windowWidth="25500" windowHeight="13455" activeTab="1" xr2:uid="{4163D5BD-C045-4706-9AC7-40FDC645494C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{4163D5BD-C045-4706-9AC7-40FDC645494C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="1">Sheet2!$F$97</definedName>
-    <definedName name="_ftnref1" localSheetId="1">Sheet2!$G$85</definedName>
+    <definedName name="_ftn1" localSheetId="1">Sheet2!$F$43</definedName>
+    <definedName name="_ftnref1" localSheetId="1">Sheet2!$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="142">
   <si>
     <t>1.  A graduating level capstone experience which includes analysis, synthesis and critical evaluation, resulting in a defined output</t>
   </si>
@@ -818,15 +818,6 @@
       </rPr>
       <t>Financial literacy in the context of developing commercial awareness</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. A graduating level capstone experience which includes the analysis and critical evaluation of data within an independently produced piece of work </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attributes </t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>The capstone experience tackles a central scientific question or issue in depth, which the students take ownership of. All sections of the capstone experience should relate to the same issue rather than being a collection of unrelated essays. The capstone experience must be the pinnacle of the course, drawing on and extending the students’ learning at previous levels. It should be a first-hand experience of performing science. The Society accepts that research is a collaborative process (e.g. between student and supervisor) but the contribution of individual students must be identifiable and assessable.</t>
@@ -922,9 +913,6 @@
   </si>
   <si>
     <t>Students should be equipped with the knowledge of mathematics and statistical approaches needed to handle variation at different levels, especially with regard to the greatly increased amount of data being generated by modern laboratory and computing techniques. Students should understand the statistical aspects of experimental procedures, encompassing the analysis of collected data, the design and analysis of studies, the development of calibration and analysis techniques, and the robustness of data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Specific skills and knowledge appropriate to the degree title </t>
   </si>
   <si>
     <r>
@@ -950,173 +938,22 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">6. Developing creativity and enterprise </t>
-  </si>
-  <si>
-    <t>The RSB recognises the importance of creating environments that support and promote the development of creativity, enterprise and entrepreneurship with our primary focus being on the experiential creative and innovative side, as being of key value to all graduates in their future employment. Creativity requires the development of approaches to solving problems, for thinking</t>
-  </si>
-  <si>
-    <t>‘outside the box’ – more usually recognised through contributions in the arts, it is also a skill required to research and solve scientific problems, and should be taught in that context, providing key transferable employability skills.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">and reward such thinking </t>
-  </si>
-  <si>
-    <t>Institutions should make it clear how they promote creativity and creative problem solving, in the students’ programme of study, using techniques designed to develop individual and group creativity.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For group sessions there should be evidence that </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF003D7D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">students experience structured, constructive and inclusive </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>approaches to creative problem solving</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF003D7D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>. When these activities are assessed, emphasis should be placed on students demonstrating how they have engaged with techniques designed to promote creativity in individuals, and the extent of their participation in group sessions. As an example for the former, students could be asked how they have utilised a specific technique during creative problem solving. Students should not be awarded marks solely on the basis of coming up with novel ideas, as this is frequently an unrealistic expectation.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">ii. Graduates are expected to have an understanding, embedded in the teaching of their subject(s), of the following concepts (a-e): </t>
   </si>
   <si>
-    <t xml:space="preserve">As well as an environment which promotes enterprise and entrepreneurship, there are some key learning points which students should be exposed to in order to aid their understanding of the post-degree work environment.  </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This learning </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF003D7D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>should not solely be in addition to current curricula</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF003D7D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, which would lead to student overload, but should look at current curricula and approaches to see how they can be adapted to address the skills and knowledge cited.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">a. A contextualised learning experience using real-world scenarios to gain better alignment with expected key </t>
-  </si>
-  <si>
-    <t xml:space="preserve">employability skills </t>
-  </si>
-  <si>
     <t>Students learn through application and practice: there are many areas of the life sciences where principles can be taught by reference to "real-world" examples. This can often be done by inviting external specialist and employers to show how the basic science relates to their industry, for instances using Enterprise Masterclasses. Employers seek an awareness of the wider context and how to develop graduates' skills for that wider context, and HEIs are charged with preparing their students for that world.</t>
   </si>
   <si>
-    <t xml:space="preserve">b. The notion and value of intellectual </t>
-  </si>
-  <si>
-    <t xml:space="preserve">property </t>
-  </si>
-  <si>
     <t>Intellectual Property drives the economic engines of innovation - students should understand how IP rights work locally and more widely outside the UK, why IP is important for development, and how to exploit it, protect it, and be aware of the potential for infringement.</t>
   </si>
   <si>
-    <t>HEIs will recognise that these three areas (c, d and e) are intrinsic to scientific research and the use of that research. While detailed learning in these areas is dependent on the particular degrees being studied, all students should at least have an awareness of these different concepts as they relate to the successful translation of research to public benefit, be it commercial exploitation or social and environmental improvement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c. The importance of evaluating feasibility and impact through a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">reflective approach </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students should be able to place their work in the wider social and commercial context, and understand the value and importance of it, relative to the wider world.   </t>
-  </si>
-  <si>
-    <t>‘Feasibility’ can include concepts such as ‘Technology Readiness</t>
-  </si>
-  <si>
-    <t>Levels (TRL, see</t>
-  </si>
-  <si>
-    <r>
-      <t>https://publications.parliament.uk/pa/cm201011/cmselect/cm sctech/619/61913.htm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF003D7D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>as well as financial and public benefit aspects.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">d. The interdisciplinary </t>
-  </si>
-  <si>
-    <t xml:space="preserve">nature of enterprise </t>
-  </si>
-  <si>
-    <t>As well as scientific interdisciplinarity, students should be made aware of the different types of business culture and company sizes that exist, and their different attributes – a good example framework might be the supply chain in drug manufacture and its role and importance in delivering translational research. Enterprise is not just about business, and students should also be made aware of the “application of enterprise behaviours, attributes and competencies into the creation of cultural, social or economic value; Green entrepreneurship is where environmental problems are explored to result in a net positive impact on the natural environment using sustainable processes”.[1]</t>
-  </si>
-  <si>
     <t xml:space="preserve">e. Financial literacy in the context of developing commercial awareness </t>
   </si>
   <si>
     <t xml:space="preserve">‘Financial literacy’ is about understanding the wider value chain in business, and links strongly to feasibility (c above), relevant to commercial, social and green enterprises.  </t>
   </si>
   <si>
-    <t xml:space="preserve">[1] Enterprise and Entrepreneurship Education: Guidance for UK Higher Education Providers, January 2018, QAA </t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
     <t>subsection</t>
-  </si>
-  <si>
-    <t>Criterion_text</t>
-  </si>
-  <si>
-    <t>Section text</t>
-  </si>
-  <si>
-    <t>Criterion</t>
   </si>
   <si>
     <t>i</t>
@@ -1512,14 +1349,59 @@
     <t>Developing creativity and enterprise</t>
   </si>
   <si>
-    <t xml:space="preserve">i. Students are taught to apply and evaluate original or unconventional ideas, and to tackle problem solving using techniques designed to develop individual and group creativity, evidenced through assessment approaches which and reward such thinking recognise </t>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i. Students are taught to apply and evaluate original or unconventional ideas, and to tackle problem solving using techniques designed to develop individual and group creativity, evidenced through assessment approaches which and reward such thinking recognise and reward such thinking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c. The importance of evaluating feasibility and impact through a reflective approach </t>
+  </si>
+  <si>
+    <t>Students should be able to place their work in the wider social and commercial context, and understand the value and importance of it, relative to the wider world.  
+ ‘Feasibility’ can include concepts such as ‘Technology Readiness Levels (TRL, see https://publications.parliament.uk/pa/cm201011/cmselect/cm sctech/619/61913.htm) as well as financial and public benefit aspects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. A contextualised learning experience using real-world scenarios to gain better alignment with expected key employability skills </t>
+  </si>
+  <si>
+    <t xml:space="preserve">b. The notion and value of intellectual property </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d. The interdisciplinary nature of enterprise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEIs will recognise that these three areas (c, d and e) are intrinsic to scientific research and the use of that research. While detailed learning in these areas is dependent on the particular degrees being studied, all students should at least have an awareness of these different concepts as they relate to the successful translation of research to public benefit, be it commercial exploitation or social and environmental improvement.
+As well as scientific interdisciplinarity, students should be made aware of the different types of business culture and company sizes that exist, and their different attributes – a good example framework might be the supply chain in drug manufacture and its role and importance in delivering translational research. Enterprise is not just about business, and students should also be made aware of the “application of enterprise behaviours, attributes and competencies into the creation of cultural, social or economic value; Green entrepreneurship is where environmental problems are explored to result in a net positive impact on the natural environment using sustainable processes”.[1] Enterprise and Entrepreneurship Education: Guidance for UK Higher Education Providers, January 2018, QAA </t>
+  </si>
+  <si>
+    <t>criterion</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>criterion_text</t>
+  </si>
+  <si>
+    <t>section_text</t>
+  </si>
+  <si>
+    <t>subsection_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Institutions should make it clear how they promote creativity and creative problem solving, in the students’ programme of study, using techniques designed to develop individual and group creativity. For group sessions there should be evidence that students experience structured, constructive and inclusive approaches to creative problem solving. When these activities are assessed, emphasis should be placed on students demonstrating how they have engaged with techniques designed to promote creativity in individuals, and the extent of their participation in group sessions. As an example for the former, students could be asked how they have utilised a specific technique during creative problem solving. Students should not be awarded marks solely on the basis of coming up with novel ideas, as this is frequently an unrealistic expectation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1583,21 +1465,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF48A942"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF003D7D"/>
       <name val="Arial"/>
@@ -1612,7 +1479,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1664,41 +1531,6 @@
       <left style="medium">
         <color rgb="FF48A942"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF48A942"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF48A942"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF48A942"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF48A942"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF48A942"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF48A942"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF48A942"/>
-      </left>
       <right style="medium">
         <color rgb="FF48A942"/>
       </right>
@@ -1720,11 +1552,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1745,31 +1576,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="10"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1781,96 +1591,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2604,1139 +2354,808 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1AC2D5-7B42-472E-8C49-A1C121690E43}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="39.5703125" customWidth="1"/>
-    <col min="6" max="6" width="88" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="75.42578125" style="20" customWidth="1"/>
     <col min="7" max="7" width="99.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="280.5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="153" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="204" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D18" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="280.5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="20" spans="1:7" ht="165.75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="G22" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="47" t="s">
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="8" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="53.25" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G25" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="306" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="G26" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="153" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="369.75" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="F28" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="204" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" ht="306" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="F29" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="F30" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
         <v>128</v>
       </c>
-      <c r="E20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" t="s">
-        <v>137</v>
-      </c>
-      <c r="E27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F32" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="29"/>
-    </row>
-    <row r="33" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="31"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" s="23"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G37" s="11"/>
+      <c r="F36" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="17" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
-      </c>
-      <c r="D39" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" t="s">
-        <v>113</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" t="s">
-        <v>142</v>
-      </c>
-      <c r="E40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>5</v>
-      </c>
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="280.5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>5</v>
-      </c>
-      <c r="B42" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" t="s">
-        <v>153</v>
-      </c>
-      <c r="F42" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>5</v>
-      </c>
-      <c r="B43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" t="s">
-        <v>154</v>
-      </c>
-      <c r="F43" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="44" spans="1:7" ht="344.25" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F44" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="1:7" ht="293.25" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" t="s">
-        <v>142</v>
-      </c>
-      <c r="E45" t="s">
-        <v>155</v>
-      </c>
-      <c r="F45" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F46" s="48"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="1:7" ht="408" x14ac:dyDescent="0.25">
-      <c r="E47" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F48" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F49" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="G49" s="31"/>
-    </row>
-    <row r="50" spans="1:7" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>6</v>
-      </c>
-      <c r="B50" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F50" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="G50" s="40"/>
-    </row>
-    <row r="51" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>6</v>
-      </c>
-      <c r="F51" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" s="42"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G52" s="23"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F53" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F56" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s">
-        <v>95</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F58" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F59" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F60" s="15"/>
-      <c r="G60" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F61" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F62" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F63" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="F64" s="14"/>
-      <c r="G64" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F65" s="15"/>
-      <c r="G65" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F66" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" t="s">
-        <v>96</v>
-      </c>
-      <c r="F67" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F68" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F69" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G69" s="11"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F70" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>6</v>
-      </c>
-      <c r="B71" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" t="s">
-        <v>96</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G71" s="24"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F72" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G72" s="24"/>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F73" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G73" s="26"/>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F74" s="34"/>
-      <c r="G74" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F75" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="G75" s="44"/>
-    </row>
-    <row r="76" spans="1:7" ht="318.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F76" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="G76" s="40"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F77" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="G77" s="33"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F78" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G78" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F79" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G79" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F80" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F81" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" spans="6:7" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="F82" s="14"/>
-      <c r="G82" s="35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="83" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F83" s="15"/>
-      <c r="G83" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F84" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="6:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="F85" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G85" s="36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F86" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G86" s="17"/>
-    </row>
-    <row r="87" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F87" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G87" s="11"/>
-    </row>
-    <row r="88" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F88" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G88" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="6:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F89" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="G89" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F90" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="G90" s="11"/>
-    </row>
-    <row r="91" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F91" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F93" s="45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F94" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="6:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="F97" s="46" t="s">
-        <v>89</v>
-      </c>
+      <c r="F38" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G85" location="_ftn1" display="_ftn1" xr:uid="{43C25CE2-55D8-4C5B-9D1A-D5A58D044A5B}"/>
-    <hyperlink ref="F97" location="_ftnref1" display="_ftnref1" xr:uid="{026B2642-F1C4-44B1-BFA4-00FDAA236066}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>